<commit_message>
Update Cloud Labs Login Credentials - Splunk (B3) - 09-13 June 2025 - BOA.xlsx
</commit_message>
<xml_diff>
--- a/Cloud Labs Login Credentials - Splunk (B3) - 09-13 June 2025 - BOA.xlsx
+++ b/Cloud Labs Login Credentials - Splunk (B3) - 09-13 June 2025 - BOA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\OneDrive - palmeto.co.in\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VK_GIT\BOA_SPLK_09_06_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC5852C-2138-42A2-83D6-B9DAD7068508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9B01AB3-B9D1-480C-B3A6-141E74D5E368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud Labs Creds 09-13 Jun 2025" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
   <si>
     <t>Username</t>
   </si>
@@ -228,6 +226,93 @@
   </si>
   <si>
     <t>Splunk-Trainer</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>http://34.229.126.65:8000/en-US/app/launcher/home</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>user4</t>
+  </si>
+  <si>
+    <t>user5</t>
+  </si>
+  <si>
+    <t>user6</t>
+  </si>
+  <si>
+    <t>user7</t>
+  </si>
+  <si>
+    <t>user8</t>
+  </si>
+  <si>
+    <t>user9</t>
+  </si>
+  <si>
+    <t>user10</t>
+  </si>
+  <si>
+    <t>user11</t>
+  </si>
+  <si>
+    <t>user12</t>
+  </si>
+  <si>
+    <t>user13</t>
+  </si>
+  <si>
+    <t>user@123</t>
+  </si>
+  <si>
+    <t>http://3.91.6.251:8000/en-US/app/launcher/home</t>
+  </si>
+  <si>
+    <t>user14</t>
+  </si>
+  <si>
+    <t>user15</t>
+  </si>
+  <si>
+    <t>user16</t>
+  </si>
+  <si>
+    <t>user17</t>
+  </si>
+  <si>
+    <t>user18</t>
+  </si>
+  <si>
+    <t>user19</t>
+  </si>
+  <si>
+    <t>user20</t>
+  </si>
+  <si>
+    <t>user21</t>
+  </si>
+  <si>
+    <t>user22</t>
+  </si>
+  <si>
+    <t>user23</t>
+  </si>
+  <si>
+    <t>user24</t>
+  </si>
+  <si>
+    <t>user25</t>
   </si>
 </sst>
 </file>
@@ -852,7 +937,7 @@
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -877,6 +962,16 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -908,16 +1003,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1067,9 +1153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1107,7 +1193,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1213,7 +1299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1355,7 +1441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1363,70 +1449,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="19.2" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42" style="3" customWidth="1"/>
     <col min="3" max="3" width="22" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="3"/>
+    <col min="4" max="4" width="22.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="3"/>
+    <col min="6" max="6" width="54.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" spans="1:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="23"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-    </row>
-    <row r="5" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="20"/>
+      <c r="D4" s="21"/>
+    </row>
+    <row r="5" spans="1:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
@@ -1439,8 +1529,17 @@
       <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1454,8 +1553,17 @@
         <v>3</v>
       </c>
       <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -1468,8 +1576,17 @@
       <c r="D8" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>3</v>
       </c>
@@ -1482,8 +1599,17 @@
       <c r="D9" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>4</v>
       </c>
@@ -1497,8 +1623,17 @@
         <v>3</v>
       </c>
       <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1511,8 +1646,17 @@
       <c r="D11" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1525,8 +1669,17 @@
       <c r="D12" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>7</v>
       </c>
@@ -1539,8 +1692,17 @@
       <c r="D13" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>8</v>
       </c>
@@ -1553,8 +1715,17 @@
       <c r="D14" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>9</v>
       </c>
@@ -1567,8 +1738,17 @@
       <c r="D15" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>10</v>
       </c>
@@ -1581,8 +1761,17 @@
       <c r="D16" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F16" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>11</v>
       </c>
@@ -1595,8 +1784,17 @@
       <c r="D17" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H17" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="5">
         <v>12</v>
       </c>
@@ -1609,8 +1807,17 @@
       <c r="D18" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H18" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>13</v>
       </c>
@@ -1623,8 +1830,17 @@
       <c r="D19" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>14</v>
       </c>
@@ -1637,8 +1853,17 @@
       <c r="D20" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H20" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>15</v>
       </c>
@@ -1651,8 +1876,17 @@
       <c r="D21" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>16</v>
       </c>
@@ -1665,8 +1899,17 @@
       <c r="D22" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H22" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>17</v>
       </c>
@@ -1679,8 +1922,17 @@
       <c r="D23" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H23" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>18</v>
       </c>
@@ -1693,8 +1945,17 @@
       <c r="D24" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F24" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>19</v>
       </c>
@@ -1707,8 +1968,17 @@
       <c r="D25" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H25" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>20</v>
       </c>
@@ -1721,8 +1991,17 @@
       <c r="D26" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F26" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H26" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5">
         <v>21</v>
       </c>
@@ -1735,8 +2014,17 @@
       <c r="D27" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F27" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5">
         <v>22</v>
       </c>
@@ -1749,8 +2037,17 @@
       <c r="D28" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>23</v>
       </c>
@@ -1763,8 +2060,17 @@
       <c r="D29" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5">
         <v>24</v>
       </c>
@@ -1775,8 +2081,17 @@
       <c r="D30" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H30" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>25</v>
       </c>
@@ -1787,18 +2102,27 @@
       <c r="D31" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="21">
+      <c r="F31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H31" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A32" s="11">
         <v>26</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D32" s="24" t="s">
+      <c r="D32" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1816,8 +2140,26 @@
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{CBABEBDE-96BB-4278-997B-D5D704F23484}"/>
+    <hyperlink ref="H9" r:id="rId2" xr:uid="{4C4632E3-8A20-4DC7-B706-98E9D385FD5E}"/>
+    <hyperlink ref="H11" r:id="rId3" xr:uid="{93FFB266-2EDC-4675-8DFA-C5936478F570}"/>
+    <hyperlink ref="H14" r:id="rId4" xr:uid="{61F06845-080B-4E88-9AF5-DDBC6695A3C2}"/>
+    <hyperlink ref="H17" r:id="rId5" xr:uid="{A83A3DE3-7DAF-44BE-AB2D-C444D1BD78F9}"/>
+    <hyperlink ref="H12" r:id="rId6" xr:uid="{70859010-7114-4D3A-9764-EEC5A0BF5D25}"/>
+    <hyperlink ref="H15" r:id="rId7" xr:uid="{31C169A7-03C4-437E-B667-8C296D0FFE06}"/>
+    <hyperlink ref="H18" r:id="rId8" xr:uid="{10FC03A1-96AE-4BAC-9E02-75B2DFFBAB14}"/>
+    <hyperlink ref="H20" r:id="rId9" xr:uid="{8275296F-DCDD-4FF6-B752-D1FEB79BE9F6}"/>
+    <hyperlink ref="H26" r:id="rId10" xr:uid="{2F66F06A-D912-4AB6-9F29-220D2394FA4E}"/>
+    <hyperlink ref="H23" r:id="rId11" xr:uid="{9A7E2594-407D-4D50-8ED6-25D81C1BC4AC}"/>
+    <hyperlink ref="H29" r:id="rId12" xr:uid="{ECD6C551-BC55-4638-AE4D-D250FFBB0722}"/>
+    <hyperlink ref="H21" r:id="rId13" xr:uid="{7C73E00C-543B-4054-958E-5BF0C069B4AA}"/>
+    <hyperlink ref="H27" r:id="rId14" xr:uid="{C20CDEF0-9963-43CD-9165-30A02FF50DED}"/>
+    <hyperlink ref="H24" r:id="rId15" xr:uid="{C8E9B3A8-6591-401B-996F-30F42F5B442A}"/>
+    <hyperlink ref="H30" r:id="rId16" xr:uid="{C0FCDEA0-29AC-47BE-BE14-2C7694262F1A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId17"/>
+  <drawing r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>